<commit_message>
changes done to excel file
</commit_message>
<xml_diff>
--- a/src/main/java/com/jobget/testdata/data.xlsx
+++ b/src/main/java/com/jobget/testdata/data.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\backup\MyWorkspace\JobGetAssignment\src\main\java\com\jobget\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyWorkspace\JobGetAssignment\src\main\java\com\jobget\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED30CB6-3548-44A9-B62D-92018159218C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4334FD-E6F8-4B54-8647-C992F2CBB955}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{07CC0909-41E2-4388-AC07-C4F1E580B8F0}"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginDetails" sheetId="2" r:id="rId1"/>
-    <sheet name="EmployerDetails" sheetId="1" r:id="rId2"/>
+    <sheet name="EmployerDetails" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginDetails" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -35,13 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
-  <si>
-    <t>test123</t>
-  </si>
-  <si>
-    <t>test456</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>FirstName</t>
   </si>
@@ -64,7 +58,34 @@
     <t>India</t>
   </si>
   <si>
-    <t>test@abc.com</t>
+    <t>automationuser1@gmail.com</t>
+  </si>
+  <si>
+    <t>automation</t>
+  </si>
+  <si>
+    <t>user2</t>
+  </si>
+  <si>
+    <t>automationuser2@gmail.com</t>
+  </si>
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>Company Website</t>
+  </si>
+  <si>
+    <t>AutomationTesting</t>
+  </si>
+  <si>
+    <t>AutomationUser</t>
+  </si>
+  <si>
+    <t>MobileNumber</t>
+  </si>
+  <si>
+    <t>CountryCode</t>
   </si>
 </sst>
 </file>
@@ -110,7 +131,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -133,12 +154,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -154,6 +186,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -469,113 +510,82 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16BFBEE9-F493-4C37-BA03-B61F1A86D8D9}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F17BD4B2-3A86-4386-8050-58F70F0ED968}">
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.54296875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="30.90625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.90625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="21.26953125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="19.7265625" customWidth="1"/>
+    <col min="1" max="1" width="18.453125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.54296875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.6328125" customWidth="1"/>
+    <col min="6" max="6" width="19.90625" customWidth="1"/>
+    <col min="7" max="7" width="17.7265625" customWidth="1"/>
+    <col min="8" max="8" width="12.81640625" customWidth="1"/>
+    <col min="9" max="9" width="16.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="8">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{2610EC44-7A03-4589-B3F2-62E7772760F0}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F17BD4B2-3A86-4386-8050-58F70F0ED968}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="27.54296875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="30.90625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.90625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="21.26953125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="19.7265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>8</v>
+      <c r="I2" s="8">
+        <v>8579904918</v>
       </c>
     </row>
   </sheetData>
@@ -585,4 +595,49 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16BFBEE9-F493-4C37-BA03-B61F1A86D8D9}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A5:A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31.54296875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21.26953125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{A8D3D21E-334C-44F3-9CD5-14AC3CA1FD95}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added code for csv
</commit_message>
<xml_diff>
--- a/src/main/java/com/jobget/testdata/data.xlsx
+++ b/src/main/java/com/jobget/testdata/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyWorkspace\JobGetAssignment\src\main\java\com\jobget\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4334FD-E6F8-4B54-8647-C992F2CBB955}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EC506C-99FE-457C-8644-E23C08C0793D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{07CC0909-41E2-4388-AC07-C4F1E580B8F0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{07CC0909-41E2-4388-AC07-C4F1E580B8F0}"/>
   </bookViews>
   <sheets>
     <sheet name="EmployerDetails" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>FirstName</t>
   </si>
@@ -58,9 +58,6 @@
     <t>India</t>
   </si>
   <si>
-    <t>automationuser1@gmail.com</t>
-  </si>
-  <si>
     <t>automation</t>
   </si>
   <si>
@@ -86,6 +83,12 @@
   </si>
   <si>
     <t>CountryCode</t>
+  </si>
+  <si>
+    <t>Test@123!</t>
+  </si>
+  <si>
+    <t>automationuser4846@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -513,7 +516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F17BD4B2-3A86-4386-8050-58F70F0ED968}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -547,27 +550,27 @@
         <v>5</v>
       </c>
       <c r="F1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="H1" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
@@ -576,10 +579,10 @@
         <v>6</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="H2" s="8">
         <v>1</v>
@@ -601,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16BFBEE9-F493-4C37-BA03-B61F1A86D8D9}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A5:A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -623,12 +626,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>6</v>
@@ -637,6 +640,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{A8D3D21E-334C-44F3-9CD5-14AC3CA1FD95}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{9098959B-8BA4-4371-A936-B97C552B043D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>